<commit_message>
RepMeth migrated to Playwright
</commit_message>
<xml_diff>
--- a/src/resources/data/testData.xlsx
+++ b/src/resources/data/testData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dpaluri\Desktop\IA_test\AutomationCypress\src\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsmyk\Playwright\Major\AutomationCypress\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12595819-D583-4647-AA91-941674CF51CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA916A7B-A0EB-4631-B5DF-889E4AA80D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="9720" tabRatio="734" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="64080" yWindow="1530" windowWidth="21600" windowHeight="11385" tabRatio="734" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
     <sheet name="CreateFirm" sheetId="12" r:id="rId2"/>
     <sheet name="LoginTest" sheetId="2" r:id="rId3"/>
+    <sheet name="AddEditDelete_ReportingMethods" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>TestID</t>
   </si>
@@ -93,6 +94,36 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>ReportingMethodName</t>
+  </si>
+  <si>
+    <t>CostAccountingMethod</t>
+  </si>
+  <si>
+    <t>DateType</t>
+  </si>
+  <si>
+    <t>FIFO</t>
+  </si>
+  <si>
+    <t>Settle Date</t>
+  </si>
+  <si>
+    <t>EditedReportingMethodName</t>
+  </si>
+  <si>
+    <t>Testing Add-Edit-Delete function for Reporing Methods</t>
+  </si>
+  <si>
+    <t>RM_AddEditDelete</t>
+  </si>
+  <si>
+    <t>Test FIFO Method 2</t>
+  </si>
+  <si>
+    <t>Test FIFO Method Edited 2</t>
   </si>
 </sst>
 </file>
@@ -130,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,11 +169,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -150,6 +196,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +826,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,6 +835,7 @@
     <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -828,4 +880,68 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36701B2-6574-42D0-8268-CAE67AF25034}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>